<commit_message>
100ms Basic Timer example
</commit_message>
<xml_diff>
--- a/Docs/Common/timer_period_caclulation.xlsx
+++ b/Docs/Common/timer_period_caclulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practise\GitHub\ESW\Docs\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62CC2D66-2585-4956-8F7D-B2B9DCB24F9B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AE3B8F-551D-43FC-856E-90CFA01A033F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48000" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Example of Output capture Timer 4 Channels
</commit_message>
<xml_diff>
--- a/Docs/Common/timer_period_caclulation.xlsx
+++ b/Docs/Common/timer_period_caclulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practise\GitHub\ESW\Docs\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2AE3B8F-551D-43FC-856E-90CFA01A033F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144B77AD-66D9-423B-868D-E473EC352A87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48000" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -576,7 +576,7 @@
         <v>10</v>
       </c>
       <c r="B26">
-        <v>1</v>
+        <v>1000</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -585,7 +585,7 @@
       </c>
       <c r="B27">
         <f>1/B26</f>
-        <v>1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -594,7 +594,7 @@
       </c>
       <c r="B29">
         <f>(B27/B24)/2</f>
-        <v>12500000</v>
+        <v>12500</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
PWM Timer 4 Channels with various duty cycles.
</commit_message>
<xml_diff>
--- a/Docs/Common/timer_period_caclulation.xlsx
+++ b/Docs/Common/timer_period_caclulation.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Practise\GitHub\ESW\Docs\Common\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{144B77AD-66D9-423B-868D-E473EC352A87}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{329D2CF8-A59B-4459-A2FD-EFABBEB9193D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="48000" yWindow="0" windowWidth="19200" windowHeight="15600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -485,7 +485,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,7 +505,7 @@
         <v>0</v>
       </c>
       <c r="B4">
-        <v>16000000</v>
+        <v>50000000</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
@@ -513,7 +513,7 @@
         <v>1</v>
       </c>
       <c r="B6">
-        <v>24</v>
+        <v>4</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
@@ -522,7 +522,7 @@
       </c>
       <c r="B8">
         <f>B4/(B6+1)</f>
-        <v>640000</v>
+        <v>10000000</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
@@ -531,7 +531,7 @@
       </c>
       <c r="B10">
         <f>1/B8</f>
-        <v>1.5625000000000001E-6</v>
+        <v>9.9999999999999995E-8</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
@@ -540,7 +540,7 @@
       </c>
       <c r="B12">
         <f>B14/B10</f>
-        <v>64000</v>
+        <v>10000</v>
       </c>
       <c r="C12" t="s">
         <v>12</v>
@@ -551,7 +551,7 @@
         <v>5</v>
       </c>
       <c r="B14">
-        <v>0.1</v>
+        <v>1E-3</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">

</xml_diff>